<commit_message>
Fix duplicate taxon names created by Split-then-NEw or New-then-New errors in spreadsheet.
</commit_message>
<xml_diff>
--- a/7d.REPORT.QC check for duplicate taxon names.sql.xlsx
+++ b/7d.REPORT.QC check for duplicate taxon names.sql.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Box Sync\ictvonline\ICTV_update\2017_updates\2017 MSL31.ICTV2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\client\github\ICTVonlineDbLoad\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Unnamed genus" sheetId="2" r:id="rId2"/>
     <sheet name="Species=Genus" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="80">
   <si>
     <t>New,</t>
   </si>
@@ -34,48 +34,21 @@
     <t>Ratification_1998</t>
   </si>
   <si>
-    <t>Unassigned;Unassigned;Unassigned;Tymovirus;</t>
-  </si>
-  <si>
-    <t>Chayote mosaic virus</t>
-  </si>
-  <si>
     <t>ICTV 7th Report</t>
   </si>
   <si>
     <t>Abolished,</t>
   </si>
   <si>
-    <t>2002.P108-109.Geminiviridae</t>
-  </si>
-  <si>
-    <t>Unassigned;Geminiviridae;Unassigned;Begomovirus;</t>
-  </si>
-  <si>
-    <t>ICTV 8th Report</t>
-  </si>
-  <si>
     <t>Renamed,</t>
   </si>
   <si>
-    <t>2003.P013-014.Tymovirus</t>
-  </si>
-  <si>
-    <t>Unassigned;Tymoviridae;Unassigned;Tymovirus;</t>
-  </si>
-  <si>
     <t>NULL</t>
   </si>
   <si>
-    <t>Chayote yellow mosaic virus</t>
-  </si>
-  <si>
     <t>Moved,</t>
   </si>
   <si>
-    <t>Tymovirales;Tymoviridae;Unassigned;Tymovirus;</t>
-  </si>
-  <si>
     <t>prev_tags</t>
   </si>
   <si>
@@ -97,12 +70,6 @@
     <t>next_tags</t>
   </si>
   <si>
-    <t>prev_change</t>
-  </si>
-  <si>
-    <t>next_change</t>
-  </si>
-  <si>
     <t>next_lineage</t>
   </si>
   <si>
@@ -212,13 +179,100 @@
   </si>
   <si>
     <t>2015.015a-aaD.A.v2.Polyomaviridae_rev</t>
+  </si>
+  <si>
+    <t>just this MSL</t>
+  </si>
+  <si>
+    <t>Betanucleorhabdovirus</t>
+  </si>
+  <si>
+    <t>PROBLEM!</t>
+  </si>
+  <si>
+    <t>Riboviria;Betanucleorhabdovirus</t>
+  </si>
+  <si>
+    <t>Riboviria;Orthornavirae;Negarnaviricota;Haploviricotina;Monjiviricetes;Mononegavirales;Rhabdoviridae;Betanucleorhabdovirus</t>
+  </si>
+  <si>
+    <t>Cressdnaviricota</t>
+  </si>
+  <si>
+    <t>Monodnaviria;Shotokuvirae;Cressdnaviricota</t>
+  </si>
+  <si>
+    <t>Alphanucleorhabdovirus</t>
+  </si>
+  <si>
+    <t>Riboviria;Alphanucleorhabdovirus</t>
+  </si>
+  <si>
+    <t>Riboviria;Orthornavirae;Negarnaviricota;Haploviricotina;Monjiviricetes;Mononegavirales;Rhabdoviridae;Alphanucleorhabdovirus</t>
+  </si>
+  <si>
+    <t>Tubulavirales</t>
+  </si>
+  <si>
+    <t>Monodnaviria;Loebvirae;Hofneiviricota;Faserviricetes;Tubulavirales</t>
+  </si>
+  <si>
+    <t>Hamaparvovirinae</t>
+  </si>
+  <si>
+    <t>Monodnaviria;Shotokuvirae;Cossaviricota;Quintoviricetes;Piccovirales;Parvoviridae;Hamaparvovirinae</t>
+  </si>
+  <si>
+    <t>Plectroviridae</t>
+  </si>
+  <si>
+    <t>Monodnaviria;Loebvirae;Hofneiviricota;Faserviricetes;Tubulavirales;Plectroviridae</t>
+  </si>
+  <si>
+    <t>scope</t>
+  </si>
+  <si>
+    <t>msl_release_num</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>duplicate taxon names</t>
+  </si>
+  <si>
+    <t>min_lineage</t>
+  </si>
+  <si>
+    <t>max_lineage</t>
+  </si>
+  <si>
+    <t>FIX</t>
+  </si>
+  <si>
+    <t>new(1015) and new(1014) with diff parents. Use 1014 (Faserviricetes)</t>
+  </si>
+  <si>
+    <t>new(450) and new(449) with diff parents. Use 449 (Shotokuvirae)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new(166) and new(1018). Both correct, though differ on molecule (ssDNA vs ssDNA(+)). </t>
+  </si>
+  <si>
+    <t>split (814) and new(815). Use split, fix parent.</t>
+  </si>
+  <si>
+    <t>split (373.1) and new(394). Use split, fix parent.</t>
+  </si>
+  <si>
+    <t>split(814.1)  and new (825). Use split, fix parent.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +302,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -269,8 +330,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -302,20 +362,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -594,323 +653,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A7" activeCellId="2" sqref="A3 A5 A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="94.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="119" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>23</v>
+    <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
+        <v>71</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C2">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
+        <v>54</v>
+      </c>
+      <c r="H2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4">
-        <v>22</v>
+        <v>51</v>
+      </c>
+      <c r="C3">
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
+        <v>56</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="4">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>3</v>
+        <v>51</v>
+      </c>
+      <c r="C4">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="H4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
       <c r="C5">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
+        <v>61</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="C6">
-        <v>23</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
       <c r="C7">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3</v>
+        <v>65</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C8">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <v>25</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12">
-        <v>26</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>27</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <v>27</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <v>28</v>
-      </c>
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16">
-        <v>28</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17">
-        <v>29</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18">
-        <v>29</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19">
-        <v>30</v>
-      </c>
-      <c r="D19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <v>30</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21">
-        <v>31</v>
-      </c>
-      <c r="D21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22">
-        <v>31</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>13</v>
+        <v>66</v>
+      </c>
+      <c r="H7" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G22">
-    <sortCondition ref="C2:C22"/>
-    <sortCondition ref="E2:E22"/>
+  <sortState ref="B2:H22">
+    <sortCondition ref="D2:D22"/>
+    <sortCondition ref="F2:F22"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
@@ -939,28 +885,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -968,25 +914,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -994,19 +940,19 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1014,25 +960,25 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1040,25 +986,25 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1066,48 +1012,48 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1137,28 +1083,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1166,131 +1112,131 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="4">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>44</v>
+        <v>32</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="4">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>44</v>
+      <c r="D3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="4">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>44</v>
+        <v>32</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H4" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="4">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>44</v>
+      <c r="D5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="4">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>44</v>
+        <v>32</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="4">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2">
         <v>3</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>44</v>
+      <c r="D7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H7" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1298,657 +1244,657 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>54</v>
+      <c r="E9" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" t="s">
         <v>46</v>
-      </c>
-      <c r="B10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="4">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>54</v>
+        <v>42</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H11" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="4">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2">
         <v>2</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>54</v>
+      <c r="D12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H12" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="4">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>54</v>
+        <v>42</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H13" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="4">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2">
         <v>3</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>54</v>
+      <c r="D14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="G14" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H14" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H15" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H16" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H17" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C18">
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H18" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C19">
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H19" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C20">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H20" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C21">
         <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H21" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C22">
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H22" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C23">
         <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H23" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C24">
         <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F24" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H24" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C25">
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E25" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H25" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C26">
         <v>15</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E26" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H26" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C27">
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E27" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F27" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H27" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C28">
         <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E28" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F28" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G28" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H28" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C29">
         <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E29" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H29" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C30">
         <v>19</v>
       </c>
       <c r="D30" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E30" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F30" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H30" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C31">
         <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E31" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H31" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C32">
         <v>21</v>
       </c>
       <c r="D32" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E32" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F32" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H32" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C33">
         <v>22</v>
       </c>
       <c r="D33" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E33" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F33" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H33" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C34">
         <v>23</v>
       </c>
       <c r="D34" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E34" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F34" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H34" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C35">
         <v>24</v>
       </c>
       <c r="D35" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E35" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H35" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C36">
         <v>25</v>
       </c>
       <c r="D36" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E36" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F36" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H36" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C37">
         <v>26</v>
       </c>
       <c r="D37" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E37" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F37" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H37" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C38">
         <v>27</v>
       </c>
       <c r="D38" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F38" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C39">
         <v>28</v>
       </c>
       <c r="D39" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E39" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F39" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H39" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C40">
         <v>29</v>
       </c>
       <c r="D40" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E40" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F40" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G40" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H40" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>